<commit_message>
1 Bug has been added
</commit_message>
<xml_diff>
--- a/Bug_Report.xlsx
+++ b/Bug_Report.xlsx
@@ -5,16 +5,16 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Farah\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mazmy\Documents\GitHub\Project\Learning-hub\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7760"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511" concurrentCalc="0"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="28">
   <si>
     <t>ID</t>
   </si>
@@ -90,6 +90,31 @@
     <t xml:space="preserve">1- login as admin with vaild username and password 
 2- a request pages should be  loaded with the appearance of table that inculde   title , Date uploaded , uploaded by , status
 3-click on notificaton button </t>
+  </si>
+  <si>
+    <t>Stopper</t>
+  </si>
+  <si>
+    <t>The sign up button redirects to Server Error page</t>
+  </si>
+  <si>
+    <t>1-Open the project file on Visual Studio
+2- Run the project on Google Chrome or Firefox browsers
+3- Click on Register
+4- Fill in the form
+5-Click on Submit button</t>
+  </si>
+  <si>
+    <t>The user will be redirected to the home page after creating the account</t>
+  </si>
+  <si>
+    <t>The user is redirected to Server Error page</t>
+  </si>
+  <si>
+    <t>Opened</t>
+  </si>
+  <si>
+    <t>RM_3</t>
   </si>
 </sst>
 </file>
@@ -205,30 +230,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -246,6 +252,15 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -528,84 +543,84 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z4"/>
+  <dimension ref="A1:Z11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="23.7109375" style="9" customWidth="1"/>
-    <col min="2" max="2" width="50.28515625" customWidth="1"/>
-    <col min="3" max="3" width="45.7109375" customWidth="1"/>
-    <col min="4" max="4" width="34.5703125" customWidth="1"/>
-    <col min="5" max="6" width="32.28515625" customWidth="1"/>
-    <col min="7" max="7" width="12.7109375" customWidth="1"/>
-    <col min="8" max="8" width="27.85546875" customWidth="1"/>
+    <col min="1" max="1" width="23.7265625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="50.26953125" customWidth="1"/>
+    <col min="3" max="3" width="45.7265625" customWidth="1"/>
+    <col min="4" max="4" width="34.54296875" customWidth="1"/>
+    <col min="5" max="6" width="32.26953125" customWidth="1"/>
+    <col min="7" max="7" width="12.7265625" customWidth="1"/>
+    <col min="8" max="8" width="27.81640625" customWidth="1"/>
     <col min="9" max="9" width="41" customWidth="1"/>
-    <col min="10" max="10" width="35.5703125" customWidth="1"/>
+    <col min="10" max="10" width="35.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" s="13" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="10" t="s">
+    <row r="1" spans="1:26" s="6" customFormat="1" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="11" t="s">
+      <c r="F1" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="G1" s="11" t="s">
+      <c r="G1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="11" t="s">
+      <c r="H1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="11" t="s">
+      <c r="I1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="10" t="s">
+      <c r="J1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="12"/>
-      <c r="L1" s="12"/>
-      <c r="M1" s="12"/>
-      <c r="N1" s="12"/>
-      <c r="O1" s="12"/>
-      <c r="P1" s="12"/>
-      <c r="Q1" s="12"/>
-      <c r="R1" s="12"/>
-      <c r="S1" s="12"/>
-      <c r="T1" s="12"/>
-      <c r="U1" s="12"/>
-      <c r="V1" s="12"/>
-      <c r="W1" s="12"/>
-      <c r="X1" s="12"/>
-      <c r="Y1" s="12"/>
-      <c r="Z1" s="12"/>
+      <c r="K1" s="5"/>
+      <c r="L1" s="5"/>
+      <c r="M1" s="5"/>
+      <c r="N1" s="5"/>
+      <c r="O1" s="5"/>
+      <c r="P1" s="5"/>
+      <c r="Q1" s="5"/>
+      <c r="R1" s="5"/>
+      <c r="S1" s="5"/>
+      <c r="T1" s="5"/>
+      <c r="U1" s="5"/>
+      <c r="V1" s="5"/>
+      <c r="W1" s="5"/>
+      <c r="X1" s="5"/>
+      <c r="Y1" s="5"/>
+      <c r="Z1" s="5"/>
     </row>
-    <row r="2" spans="1:26" s="7" customFormat="1" ht="90" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+    <row r="2" spans="1:26" s="9" customFormat="1" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A2" s="9" t="s">
         <v>10</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="14" t="s">
+      <c r="C2" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="D2" s="14" t="s">
+      <c r="D2" s="7" t="s">
         <v>18</v>
       </c>
       <c r="E2" s="1" t="s">
@@ -623,68 +638,86 @@
       <c r="I2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="J2" s="15" t="s">
+      <c r="J2" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="K2" s="4"/>
-      <c r="L2" s="4"/>
-      <c r="M2" s="4"/>
-      <c r="N2" s="4"/>
-      <c r="O2" s="4"/>
-      <c r="P2" s="4"/>
-      <c r="Q2" s="4"/>
-      <c r="R2" s="4"/>
-      <c r="S2" s="4"/>
-      <c r="T2" s="4"/>
-      <c r="U2" s="4"/>
-      <c r="V2" s="4"/>
-      <c r="W2" s="4"/>
-      <c r="X2" s="4"/>
-      <c r="Y2" s="4"/>
-      <c r="Z2" s="4"/>
+      <c r="K2" s="1"/>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1"/>
+      <c r="N2" s="1"/>
+      <c r="O2" s="1"/>
+      <c r="P2" s="1"/>
+      <c r="Q2" s="1"/>
+      <c r="R2" s="1"/>
+      <c r="S2" s="1"/>
+      <c r="T2" s="1"/>
+      <c r="U2" s="1"/>
+      <c r="V2" s="1"/>
+      <c r="W2" s="1"/>
+      <c r="X2" s="1"/>
+      <c r="Y2" s="1"/>
+      <c r="Z2" s="1"/>
     </row>
-    <row r="3" spans="1:26" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+    <row r="3" spans="1:26" s="9" customFormat="1" ht="87" x14ac:dyDescent="0.35">
+      <c r="A3" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="4"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
-      <c r="H3" s="4"/>
-      <c r="I3" s="4"/>
-      <c r="J3" s="6"/>
-      <c r="K3" s="4"/>
-      <c r="L3" s="4"/>
-      <c r="M3" s="4"/>
-      <c r="N3" s="4"/>
-      <c r="O3" s="4"/>
-      <c r="P3" s="4"/>
-      <c r="Q3" s="4"/>
-      <c r="R3" s="4"/>
-      <c r="S3" s="4"/>
-      <c r="T3" s="4"/>
-      <c r="U3" s="4"/>
-      <c r="V3" s="4"/>
-      <c r="W3" s="4"/>
-      <c r="X3" s="4"/>
-      <c r="Y3" s="4"/>
-      <c r="Z3" s="4"/>
+      <c r="B3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J3" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="K3" s="1"/>
+      <c r="L3" s="1"/>
+      <c r="M3" s="1"/>
+      <c r="N3" s="1"/>
+      <c r="O3" s="1"/>
+      <c r="P3" s="1"/>
+      <c r="Q3" s="1"/>
+      <c r="R3" s="1"/>
+      <c r="S3" s="1"/>
+      <c r="T3" s="1"/>
+      <c r="U3" s="1"/>
+      <c r="V3" s="1"/>
+      <c r="W3" s="1"/>
+      <c r="X3" s="1"/>
+      <c r="Y3" s="1"/>
+      <c r="Z3" s="1"/>
     </row>
-    <row r="4" spans="1:26" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
+    <row r="4" spans="1:26" s="9" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="9" t="s">
         <v>12</v>
       </c>
       <c r="B4" s="1"/>
-      <c r="C4" s="8"/>
-      <c r="D4" s="8"/>
-      <c r="E4" s="8"/>
+      <c r="C4" s="11"/>
+      <c r="D4" s="11"/>
+      <c r="E4" s="11"/>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
-      <c r="J4" s="6"/>
+      <c r="J4" s="8"/>
       <c r="K4" s="1"/>
       <c r="L4" s="1"/>
       <c r="M4" s="1"/>
@@ -702,6 +735,13 @@
       <c r="Y4" s="1"/>
       <c r="Z4" s="1"/>
     </row>
+    <row r="5" spans="1:26" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="6" spans="1:26" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="7" spans="1:26" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="8" spans="1:26" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="9" spans="1:26" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="10" spans="1:26" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="11" spans="1:26" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
RM bugs has been added
</commit_message>
<xml_diff>
--- a/Bug_Report.xlsx
+++ b/Bug_Report.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7760"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7760" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="RM" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="55">
   <si>
     <t>ID</t>
   </si>
@@ -57,9 +58,6 @@
   </si>
   <si>
     <t>Lhub_001</t>
-  </si>
-  <si>
-    <t>Lhub_002</t>
   </si>
   <si>
     <t>Lhub_003</t>
@@ -114,7 +112,105 @@
     <t>Opened</t>
   </si>
   <si>
-    <t>RM_3</t>
+    <t>RM_9</t>
+  </si>
+  <si>
+    <t>Fixed</t>
+  </si>
+  <si>
+    <t>RM_Bug_001</t>
+  </si>
+  <si>
+    <t>RM_Bug_002</t>
+  </si>
+  <si>
+    <t>RM_Bug_003</t>
+  </si>
+  <si>
+    <t>RM_10</t>
+  </si>
+  <si>
+    <t>RM_12</t>
+  </si>
+  <si>
+    <t>RM_13</t>
+  </si>
+  <si>
+    <t>RM_Bug_004</t>
+  </si>
+  <si>
+    <t>The system accepted blank spaces in the username field</t>
+  </si>
+  <si>
+    <t>The system accepted special character in the username field</t>
+  </si>
+  <si>
+    <t>The mandatory fields are not marked with *</t>
+  </si>
+  <si>
+    <t>1-Open the project file on Visual Studio
+2- Run the project on Google Chrome or Firefox browsers
+3- Click on Register</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The mandatory fields (username, password, confirm password, email) are marked with * </t>
+  </si>
+  <si>
+    <t>The fields mentioned are not marked with *</t>
+  </si>
+  <si>
+    <t>Low</t>
+  </si>
+  <si>
+    <t>UI</t>
+  </si>
+  <si>
+    <t>RM_2</t>
+  </si>
+  <si>
+    <t>RM_Bug_005</t>
+  </si>
+  <si>
+    <t>The system accepted an already existing username to register a new account</t>
+  </si>
+  <si>
+    <t>1-Open the project file on Visual Studio
+2- Run the project on Google Chrome or Firefox browsers
+3- Click on Register
+4- Fill in the username with "Moh amed"
+5-Click on Submit button</t>
+  </si>
+  <si>
+    <t>1-Open the project file on Visual Studio
+2- Run the project on Google Chrome or Firefox browsers
+3- Click on Register
+4- Fill in the username with "Moh@med"
+5-Click on Submit button</t>
+  </si>
+  <si>
+    <t>1-Open the project file on Visual Studio
+2- Run the project on Google Chrome or Firefox browsers
+3- Click on Register
+4- Fill in the username with an already existing one like "Mohamed92"
+5-Click on Submit button</t>
+  </si>
+  <si>
+    <t>Medium</t>
+  </si>
+  <si>
+    <t>Critical</t>
+  </si>
+  <si>
+    <t>The system refuses to submit the form as the username contains a blank space</t>
+  </si>
+  <si>
+    <t>The system refuses to submit the form as the username contains a special character</t>
+  </si>
+  <si>
+    <t>The system refuses to submit the form as the username already exists</t>
+  </si>
+  <si>
+    <t>The system submitted the new account normally without giving any errors</t>
   </si>
 </sst>
 </file>
@@ -230,7 +326,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -257,12 +353,44 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -545,8 +673,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="F1" sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -579,7 +707,7 @@
         <v>4</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G1" s="4" t="s">
         <v>5</v>
@@ -615,31 +743,31 @@
         <v>10</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="7" t="s">
-        <v>20</v>
-      </c>
       <c r="D2" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="G2" s="1" t="s">
-        <v>15</v>
-      </c>
       <c r="H2" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I2" s="1" t="s">
         <v>9</v>
       </c>
       <c r="J2" s="8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K2" s="1"/>
       <c r="L2" s="1"/>
@@ -658,62 +786,14 @@
       <c r="Y2" s="1"/>
       <c r="Z2" s="1"/>
     </row>
-    <row r="3" spans="1:26" s="9" customFormat="1" ht="87" x14ac:dyDescent="0.35">
-      <c r="A3" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C3" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="J3" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="K3" s="1"/>
-      <c r="L3" s="1"/>
-      <c r="M3" s="1"/>
-      <c r="N3" s="1"/>
-      <c r="O3" s="1"/>
-      <c r="P3" s="1"/>
-      <c r="Q3" s="1"/>
-      <c r="R3" s="1"/>
-      <c r="S3" s="1"/>
-      <c r="T3" s="1"/>
-      <c r="U3" s="1"/>
-      <c r="V3" s="1"/>
-      <c r="W3" s="1"/>
-      <c r="X3" s="1"/>
-      <c r="Y3" s="1"/>
-      <c r="Z3" s="1"/>
-    </row>
     <row r="4" spans="1:26" s="9" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A4" s="9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B4" s="1"/>
-      <c r="C4" s="11"/>
-      <c r="D4" s="11"/>
-      <c r="E4" s="11"/>
+      <c r="C4" s="10"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10"/>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
@@ -745,4 +825,274 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:Z8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="11.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.26953125" style="15" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="33.7265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.08984375" style="11" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.08984375" style="11" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.36328125" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="8.7265625" style="23"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:26" s="20" customFormat="1" ht="37" x14ac:dyDescent="0.45">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" s="19"/>
+      <c r="L1" s="19"/>
+      <c r="M1" s="19"/>
+      <c r="N1" s="19"/>
+      <c r="O1" s="19"/>
+      <c r="P1" s="19"/>
+      <c r="Q1" s="19"/>
+      <c r="R1" s="19"/>
+      <c r="S1" s="19"/>
+      <c r="T1" s="19"/>
+      <c r="U1" s="19"/>
+      <c r="V1" s="19"/>
+      <c r="W1" s="19"/>
+      <c r="X1" s="19"/>
+      <c r="Y1" s="19"/>
+      <c r="Z1" s="19"/>
+    </row>
+    <row r="2" spans="1:26" s="22" customFormat="1" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A2" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="K2" s="21"/>
+      <c r="L2" s="21"/>
+      <c r="M2" s="21"/>
+      <c r="N2" s="21"/>
+      <c r="O2" s="21"/>
+      <c r="P2" s="21"/>
+      <c r="Q2" s="21"/>
+      <c r="R2" s="21"/>
+      <c r="S2" s="21"/>
+      <c r="T2" s="21"/>
+      <c r="U2" s="21"/>
+      <c r="V2" s="21"/>
+      <c r="W2" s="21"/>
+      <c r="X2" s="21"/>
+      <c r="Y2" s="21"/>
+      <c r="Z2" s="21"/>
+    </row>
+    <row r="3" spans="1:26" s="22" customFormat="1" ht="87" x14ac:dyDescent="0.35">
+      <c r="A3" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="K3" s="21"/>
+      <c r="L3" s="21"/>
+      <c r="M3" s="21"/>
+      <c r="N3" s="21"/>
+      <c r="O3" s="21"/>
+      <c r="P3" s="21"/>
+      <c r="Q3" s="21"/>
+      <c r="R3" s="21"/>
+      <c r="S3" s="21"/>
+      <c r="T3" s="21"/>
+      <c r="U3" s="21"/>
+      <c r="V3" s="21"/>
+      <c r="W3" s="21"/>
+      <c r="X3" s="21"/>
+      <c r="Y3" s="21"/>
+      <c r="Z3" s="21"/>
+    </row>
+    <row r="4" spans="1:26" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A4" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="C4" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="D4" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="E4" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A5" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="B5" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="C5" s="16" t="s">
+        <v>47</v>
+      </c>
+      <c r="D5" s="18" t="s">
+        <v>52</v>
+      </c>
+      <c r="E5" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A6" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="B6" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="C6" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="D6" s="18" t="s">
+        <v>53</v>
+      </c>
+      <c r="E6" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="B7" s="14"/>
+    </row>
+    <row r="8" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="B8" s="14"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>